<commit_message>
update import - photo - 12:11 - 18-09-2023
</commit_message>
<xml_diff>
--- a/phpspreadsheet/files/Employee List.xlsx
+++ b/phpspreadsheet/files/Employee List.xlsx
@@ -1,30 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\THUCTAPSANXUAT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\THUCTAP\VENTECH\PROJECT\hrm\phpspreadsheet\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BC5B4D-C59B-417A-B6B3-E1453B6E7432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0974D8E-F072-4A5B-B3F4-0F12464931AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
   <si>
     <t>Employee Code</t>
   </si>
   <si>
+    <t>Photo</t>
+  </si>
+  <si>
     <t>Employee Name</t>
   </si>
   <si>
@@ -109,7 +112,7 @@
     <t>Location</t>
   </si>
   <si>
-    <t>NS01</t>
+    <t>NS04</t>
   </si>
   <si>
     <t>Trần Hoàng Lam</t>
@@ -193,7 +196,7 @@
     <t>HO CHI MINH</t>
   </si>
   <si>
-    <t>NS02</t>
+    <t>NS05</t>
   </si>
   <si>
     <t>Nguyễn Lê Trường Chinh</t>
@@ -265,7 +268,7 @@
     <t>MALAYSIA</t>
   </si>
   <si>
-    <t>NS03</t>
+    <t>NS06</t>
   </si>
   <si>
     <t>Nguyễn Nhật Linh</t>
@@ -341,12 +344,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -354,13 +357,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="5">
@@ -373,27 +376,23 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC5E0B4"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB4C7E7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -420,39 +419,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -470,6 +464,161 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>122928</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1196339</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>701040</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54054E94-8A06-9B53-222F-B79C7B6A9DAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1410708" y="243841"/>
+          <a:ext cx="1073411" cy="701039"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>122928</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1196339</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>701040</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{400D85E5-CAAE-48C8-8E4D-4521760D3B34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1410708" y="243841"/>
+          <a:ext cx="1073411" cy="701039"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>122928</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1196339</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>701040</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D120A26-2B6E-4129-A1FC-4E8A5C76167D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1410708" y="243841"/>
+          <a:ext cx="1073411" cy="701039"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -760,146 +909,144 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="18.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="52" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="31.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="16.8984375" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="28.59765625" customWidth="1"/>
+    <col min="5" max="5" width="15.59765625" customWidth="1"/>
+    <col min="6" max="6" width="7.8984375" customWidth="1"/>
+    <col min="7" max="7" width="18.09765625" customWidth="1"/>
+    <col min="8" max="8" width="16.8984375" customWidth="1"/>
+    <col min="9" max="9" width="11.69921875" customWidth="1"/>
+    <col min="10" max="10" width="20.8984375" customWidth="1"/>
+    <col min="11" max="11" width="19.59765625" customWidth="1"/>
+    <col min="12" max="12" width="16.8984375" customWidth="1"/>
+    <col min="13" max="14" width="18.09765625" customWidth="1"/>
+    <col min="15" max="15" width="15.59765625" customWidth="1"/>
+    <col min="16" max="16" width="16.8984375" customWidth="1"/>
+    <col min="17" max="17" width="18.09765625" customWidth="1"/>
+    <col min="18" max="19" width="52" customWidth="1"/>
+    <col min="20" max="20" width="24.69921875" customWidth="1"/>
+    <col min="21" max="21" width="27.296875" customWidth="1"/>
+    <col min="22" max="22" width="26" customWidth="1"/>
+    <col min="23" max="23" width="15.59765625" customWidth="1"/>
+    <col min="24" max="24" width="13.3984375" customWidth="1"/>
+    <col min="25" max="25" width="18.8984375" style="1" customWidth="1"/>
+    <col min="26" max="27" width="13" customWidth="1"/>
+    <col min="28" max="28" width="22.09765625" customWidth="1"/>
+    <col min="29" max="29" width="13" customWidth="1"/>
+    <col min="30" max="30" width="22.296875" customWidth="1"/>
+    <col min="31" max="31" width="20" customWidth="1"/>
+    <col min="32" max="32" width="14.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:32" ht="19.5" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="AF1" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" ht="60.6" customHeight="1">
       <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
         <v>30</v>
       </c>
       <c r="C2" t="s">
@@ -920,34 +1067,34 @@
       <c r="H2" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="6" t="s">
         <v>44</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="R2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>45</v>
       </c>
       <c r="S2" t="s">
@@ -965,36 +1112,36 @@
       <c r="W2" t="s">
         <v>50</v>
       </c>
-      <c r="X2" s="9">
+      <c r="X2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="10">
         <v>1</v>
       </c>
-      <c r="Y2" t="s">
-        <v>45</v>
-      </c>
       <c r="Z2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AA2" t="s">
         <v>52</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AB2" t="s">
         <v>53</v>
       </c>
       <c r="AC2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AD2" s="8" t="s">
         <v>55</v>
       </c>
       <c r="AE2" t="s">
         <v>56</v>
       </c>
+      <c r="AF2" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="3" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" ht="54.6" customHeight="1">
       <c r="A3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" t="s">
         <v>58</v>
       </c>
       <c r="C3" t="s">
@@ -1013,36 +1160,36 @@
         <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" s="8" t="s">
+      <c r="O3" s="6" t="s">
         <v>70</v>
       </c>
+      <c r="P3" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="Q3" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="R3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R3" s="8" t="s">
         <v>71</v>
       </c>
       <c r="S3" t="s">
@@ -1052,92 +1199,92 @@
         <v>73</v>
       </c>
       <c r="U3" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="V3" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="W3" t="s">
         <v>75</v>
       </c>
-      <c r="X3" s="9">
+      <c r="X3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y3" s="10">
         <v>2</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>76</v>
       </c>
       <c r="Z3" t="s">
         <v>77</v>
       </c>
       <c r="AA3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB3" s="8" t="s">
         <v>78</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>53</v>
       </c>
       <c r="AC3" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AD3" s="8" t="s">
         <v>80</v>
       </c>
       <c r="AE3" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" ht="66.599999999999994" customHeight="1">
       <c r="A4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" t="s">
         <v>82</v>
       </c>
       <c r="C4" t="s">
         <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
         <v>85</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="O4" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="P4" s="8" t="s">
+      <c r="O4" s="6" t="s">
         <v>92</v>
       </c>
+      <c r="P4" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="Q4" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="R4" t="s">
+        <v>93</v>
+      </c>
+      <c r="R4" s="8" t="s">
         <v>93</v>
       </c>
       <c r="S4" t="s">
@@ -1155,11 +1302,11 @@
       <c r="W4" t="s">
         <v>98</v>
       </c>
-      <c r="X4" s="9">
+      <c r="X4" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y4" s="10">
         <v>3</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>99</v>
       </c>
       <c r="Z4" t="s">
         <v>100</v>
@@ -1167,20 +1314,24 @@
       <c r="AA4" t="s">
         <v>101</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AB4" t="s">
         <v>102</v>
       </c>
       <c r="AC4" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AD4" s="8" t="s">
         <v>104</v>
       </c>
       <c r="AE4" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>